<commit_message>
Themen & Ansprechpersonen leicht überarbeitet und eine Navigationsebene höher geschoben
</commit_message>
<xml_diff>
--- a/themen_und_ansprechpersonen.xlsx
+++ b/themen_und_ansprechpersonen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lroesele.IVV5NET\sciebo - Röseler, Lukas (lroesele@uni-muenster.de)@uni-muenster.sciebo.de\LeaRn\MueCOS-Infomodule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E1D9D1-C80A-45F6-BB81-6D0B7089684B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3595CE36-F885-423C-BB48-0DF107C8B1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EC10942A-3D47-4CC2-9B6B-6AB99B47D6AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC10942A-3D47-4CC2-9B6B-6AB99B47D6AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="110">
   <si>
     <t>0. Übergreifend</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Große Gruppen von Forschenden arbeiten häufig international und interdisziplinär im Rahmen eines Projektes gemeinsam</t>
   </si>
   <si>
-    <t>Fördert Austausch und Zusammenarbeit, Erlaubt Untersuchung von Fragestellungen, die enorme Ressourcen benötigen</t>
-  </si>
-  <si>
     <t>MüCOS</t>
   </si>
   <si>
@@ -117,18 +114,12 @@
     <t>Personen sollten nicht aufgrund ihrer Identität oder Ansichten diskriminiert werden</t>
   </si>
   <si>
-    <t>Personengruppen werden in der Wissenschaft systematisch benachteiligt und Strukturen begünstigen Machtmissbrauch.</t>
-  </si>
-  <si>
     <t>Koordination Diversity</t>
   </si>
   <si>
     <t>https://www.uni-muenster.de/profil/diversity/consulting.html</t>
   </si>
   <si>
-    <t>1. Forschungsfragen und Forschungssplanung</t>
-  </si>
-  <si>
     <t>Präregistrierung</t>
   </si>
   <si>
@@ -141,9 +132,6 @@
     <t>Sample Size Justification</t>
   </si>
   <si>
-    <t>Die benötigte Menge an Beobachtungen wird im Vorhinein durch Überlegungen, Poweranalysen, oder Datensimulationen festgelegt</t>
-  </si>
-  <si>
     <t>Erhöht Effizienz von Forschung und Präzision von Aussagen</t>
   </si>
   <si>
@@ -192,12 +180,6 @@
     <t>Open Data</t>
   </si>
   <si>
-    <t>Forschungsdaten werden online veröffentlicht und zur Nachnutzung aufbereitet (z.B. via FAIR Kriterien und mit Codebook)</t>
-  </si>
-  <si>
-    <t>Spart Kosten (z.B. weil Daten nicht erneut erhoben werden msüsen), erleichtert kumulative Forschung</t>
-  </si>
-  <si>
     <t>Service Center for Data Management</t>
   </si>
   <si>
@@ -225,9 +207,6 @@
     <t>Reproduktion, Replikation</t>
   </si>
   <si>
-    <t>Bisherige Befunde werden erneut mit denselben oder anderen Daten geprüft</t>
-  </si>
-  <si>
     <t>Test der Robustheit und Vertrauenswürdigkeit wissenschaftlicher Befunde</t>
   </si>
   <si>
@@ -237,9 +216,6 @@
     <t>Der Quellcode von Programmen wird online veröffentlicht und andere Forschende können ihn ohne Einschränkungen weiterverwenden</t>
   </si>
   <si>
-    <t>Ermöglicht Qualitätskontrolle, verhindert vendor-lock-in</t>
-  </si>
-  <si>
     <t>3. Forschungsergebnisse veröffentlichen</t>
   </si>
   <si>
@@ -273,9 +249,6 @@
     <t>Begutachtung von Forschungsartikeln wird unabhängig von Fachzeitschriften durchgeführt</t>
   </si>
   <si>
-    <t>Verbessert Qualitätskontrolle, löst Vendor-Lock-In von Forschenden bei kommerziellen Verlagen</t>
-  </si>
-  <si>
     <t>Open Peer Review</t>
   </si>
   <si>
@@ -288,21 +261,12 @@
     <t>Open Author Contributions</t>
   </si>
   <si>
-    <t>Beiträge der an einer Forschungsleistung Beteiligten werden klar kommuniziert (z.B. via CRediT)</t>
-  </si>
-  <si>
-    <t>Klärt Verantwortlichkeiten, erleichtert Zuordnung von Leistungen (z.B. für Forschungsevaluation), verhindert Ehrenautor*innenschaften</t>
-  </si>
-  <si>
     <t>4. Forschungsergebnisse kommunizieren</t>
   </si>
   <si>
     <t>Open Science in der Lehre</t>
   </si>
   <si>
-    <t>Aspekte von Open Science werden im Rahmen von Seminaren, Vorlesungen, oder entsprechenden Prüfungsleistungen diskutiert oder vorgestellt</t>
-  </si>
-  <si>
     <t>Bereitet Lernende auf steigende Anforderungen im Wissenschaftsbetrieb vor</t>
   </si>
   <si>
@@ -361,6 +325,45 @@
   </si>
   <si>
     <t>Justiziariat Forschung, Finanzen und Infrastrukturen</t>
+  </si>
+  <si>
+    <t>Fördert Austausch und Zusammenarbeit, erlaubt Untersuchung von Fragestellungen, die enorme Ressourcen benötigen</t>
+  </si>
+  <si>
+    <t>Personengruppen werden in der Wissenschaft systematisch benachteiligt und Strukturen begünstigen Machtmissbrauch</t>
+  </si>
+  <si>
+    <t>1. Forschungsfragen und Forschungsplanung</t>
+  </si>
+  <si>
+    <t>Forschungsdaten werden online veröffentlicht und zur Nachnutzung aufbereitet (z. B. via FAIR Kriterien und mit Codebook)</t>
+  </si>
+  <si>
+    <t>Beiträge der an einer Forschungsleistung Beteiligten werden klar kommuniziert (z. B. via CRediT)</t>
+  </si>
+  <si>
+    <t>Klärt Verantwortlichkeiten, erleichtert Zuordnung von Leistungen (z. B. für Forschungsevaluation), verhindert Ehrenautor*innenschaften</t>
+  </si>
+  <si>
+    <t>Spart Kosten (z. B. weil Daten nicht erneut erhoben werden müssen), erleichtert kumulative Forschung</t>
+  </si>
+  <si>
+    <t>Aspekte von Open Science werden im Rahmen von Seminaren, Vorlesungen oder entsprechenden Prüfungsleistungen diskutiert oder vorgestellt</t>
+  </si>
+  <si>
+    <t>Die benötigte Menge an Beobachtungen wird im Vorhinein durch Überlegungen, Poweranalysen oder Datensimulationen festgelegt</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>Bisherige Befunde werden erneut mit denselben (Reproduktion) oder anderen Daten (Replikation) geprüft</t>
+  </si>
+  <si>
+    <t>Ermöglicht Qualitätskontrolle, verhindert Lock-in-Effekt (d. h. Abhängigkeit durch hohe vom Anbieter erschaffene Wechselkosten)</t>
+  </si>
+  <si>
+    <t>Verbessert Qualitätskontrolle, ermöglicht Unabhängigkeit Forschender von kommerziellen Verlagen</t>
   </si>
 </sst>
 </file>
@@ -682,9 +685,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -722,7 +725,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -828,7 +831,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -970,7 +973,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -981,7 +984,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,13 +1028,13 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1039,19 +1042,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1059,35 +1062,39 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1095,15 +1102,15 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1111,19 +1118,19 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1131,433 +1138,441 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F28" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{E735CCED-4008-41EE-AF75-8644B9FA8F1A}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{BBBA463B-DD70-45D2-B308-2BC36497FBC6}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{5CEA2F9E-26B0-4A99-978A-88B2E70DF974}"/>
-    <hyperlink ref="F7" r:id="rId4" xr:uid="{E6BE1381-3917-49D3-83AA-5C950ACA4669}"/>
-    <hyperlink ref="F9" r:id="rId5" xr:uid="{40EA15B8-999D-451E-BFCD-94A3E24E190B}"/>
-    <hyperlink ref="F12" r:id="rId6" xr:uid="{D3E42375-2333-4B02-9165-21C70ACC29BC}"/>
-    <hyperlink ref="F13" r:id="rId7" xr:uid="{E7E271A0-0764-4DAA-8016-B817D44C45A5}"/>
-    <hyperlink ref="F14" r:id="rId8" xr:uid="{D0D2DA9F-E610-4DB0-97FF-9EFE35DFA463}"/>
-    <hyperlink ref="F15" r:id="rId9" xr:uid="{E52816CE-C799-4A56-8838-D9CEB219ABEB}"/>
-    <hyperlink ref="F17" r:id="rId10" xr:uid="{D90B7FDF-FBC4-43B0-8072-F916B7BC1846}"/>
-    <hyperlink ref="F19" r:id="rId11" xr:uid="{F153F629-E347-43BA-818B-F7B41AB45DEE}"/>
-    <hyperlink ref="F21" r:id="rId12" xr:uid="{FDCF67DE-5A5E-4839-B3B5-82EE968C61F6}"/>
-    <hyperlink ref="F22" r:id="rId13" xr:uid="{E76C7729-605C-4585-8693-D93785F56D56}"/>
-    <hyperlink ref="F23" r:id="rId14" xr:uid="{68264047-0810-434A-8BBD-522B84B62636}"/>
-    <hyperlink ref="F24" r:id="rId15" xr:uid="{20FD2295-1F5B-431B-9E20-63BE4C16F975}"/>
-    <hyperlink ref="F25" r:id="rId16" xr:uid="{C50946AE-F803-466A-A19D-4F0D9C660A0F}"/>
-    <hyperlink ref="F26" r:id="rId17" xr:uid="{8CD08D74-55CF-4988-96BB-22AE1AFCF03D}"/>
-    <hyperlink ref="F27" r:id="rId18" xr:uid="{C899B877-3B0C-4725-88F8-2B2B870D4FCF}"/>
-    <hyperlink ref="F8" r:id="rId19" xr:uid="{BFC8F5EF-2A4B-4A32-8D5B-731A22F2FE01}"/>
-    <hyperlink ref="F18" r:id="rId20" xr:uid="{A019E702-31EF-4648-8E8E-349D702A6B9F}"/>
+    <hyperlink ref="F27" r:id="rId1" xr:uid="{C899B877-3B0C-4725-88F8-2B2B870D4FCF}"/>
+    <hyperlink ref="F18" r:id="rId2" xr:uid="{A019E702-31EF-4648-8E8E-349D702A6B9F}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{BFC8F5EF-2A4B-4A32-8D5B-731A22F2FE01}"/>
+    <hyperlink ref="F26" r:id="rId4" xr:uid="{8CD08D74-55CF-4988-96BB-22AE1AFCF03D}"/>
+    <hyperlink ref="F25" r:id="rId5" xr:uid="{C50946AE-F803-466A-A19D-4F0D9C660A0F}"/>
+    <hyperlink ref="F24" r:id="rId6" xr:uid="{20FD2295-1F5B-431B-9E20-63BE4C16F975}"/>
+    <hyperlink ref="F23" r:id="rId7" xr:uid="{68264047-0810-434A-8BBD-522B84B62636}"/>
+    <hyperlink ref="F22" r:id="rId8" xr:uid="{E76C7729-605C-4585-8693-D93785F56D56}"/>
+    <hyperlink ref="F21" r:id="rId9" xr:uid="{FDCF67DE-5A5E-4839-B3B5-82EE968C61F6}"/>
+    <hyperlink ref="F19" r:id="rId10" xr:uid="{F153F629-E347-43BA-818B-F7B41AB45DEE}"/>
+    <hyperlink ref="F17" r:id="rId11" xr:uid="{D90B7FDF-FBC4-43B0-8072-F916B7BC1846}"/>
+    <hyperlink ref="F15" r:id="rId12" xr:uid="{E52816CE-C799-4A56-8838-D9CEB219ABEB}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{D0D2DA9F-E610-4DB0-97FF-9EFE35DFA463}"/>
+    <hyperlink ref="F13" r:id="rId14" xr:uid="{E7E271A0-0764-4DAA-8016-B817D44C45A5}"/>
+    <hyperlink ref="F12" r:id="rId15" xr:uid="{D3E42375-2333-4B02-9165-21C70ACC29BC}"/>
+    <hyperlink ref="F9" r:id="rId16" xr:uid="{40EA15B8-999D-451E-BFCD-94A3E24E190B}"/>
+    <hyperlink ref="F7" r:id="rId17" xr:uid="{E6BE1381-3917-49D3-83AA-5C950ACA4669}"/>
+    <hyperlink ref="F5" r:id="rId18" xr:uid="{5CEA2F9E-26B0-4A99-978A-88B2E70DF974}"/>
+    <hyperlink ref="F3" r:id="rId19" xr:uid="{BBBA463B-DD70-45D2-B308-2BC36497FBC6}"/>
+    <hyperlink ref="F2" r:id="rId20" xr:uid="{E735CCED-4008-41EE-AF75-8644B9FA8F1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>

</xml_diff>